<commit_message>
ajustes ortial y su estructura
</commit_message>
<xml_diff>
--- a/Base_organizada/BBDD_Ortial/Estructura.xlsx
+++ b/Base_organizada/BBDD_Ortial/Estructura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bambooanalytics-my.sharepoint.com/personal/francisco_echeverri_wadua_com_co/Documents/Documentos/Prueba_GIT_AG/Proyecto_AulaGlobal/Base_organizada/BBDD_Ortial/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danyk\OneDrive\Documents\AulaGlobalRepo\Proyecto_AulaGlobal\Base_organizada\BBDD_Ortial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="399" documentId="8_{69FC0CEC-2304-48E1-87AE-BDBA335889A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1945E07-979F-45A8-ABCA-54336C4BF613}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6FE25E-F02D-442B-9D8C-54FCF53CD718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2085" windowWidth="19440" windowHeight="15000" activeTab="2" xr2:uid="{01EC7A51-1FAE-4D41-B894-C0ABBF3FD8AA}"/>
+    <workbookView xWindow="28680" yWindow="-870" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{01EC7A51-1FAE-4D41-B894-C0ABBF3FD8AA}"/>
   </bookViews>
   <sheets>
     <sheet name="2º" sheetId="5" r:id="rId1"/>
@@ -39,34 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Departamento</t>
-  </si>
-  <si>
-    <t>Municipio</t>
-  </si>
-  <si>
-    <t>Colegio</t>
-  </si>
-  <si>
-    <t>Sede</t>
-  </si>
-  <si>
-    <t>Género</t>
-  </si>
-  <si>
-    <t>Grado</t>
-  </si>
-  <si>
-    <t>Grupo</t>
-  </si>
-  <si>
-    <t>Jornada</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
   <si>
     <t>lectura_correctas</t>
   </si>
@@ -108,6 +81,30 @@
   </si>
   <si>
     <t>id_global</t>
+  </si>
+  <si>
+    <t>departamento</t>
+  </si>
+  <si>
+    <t>municipio</t>
+  </si>
+  <si>
+    <t>colegio</t>
+  </si>
+  <si>
+    <t>sede</t>
+  </si>
+  <si>
+    <t>genero</t>
+  </si>
+  <si>
+    <t>grado</t>
+  </si>
+  <si>
+    <t>grupo</t>
+  </si>
+  <si>
+    <t>jornada</t>
   </si>
 </sst>
 </file>
@@ -196,7 +193,28 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3B7DE413-7D9E-6242-B8EB-123B5FAF1750}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{8B9EEF82-AB34-084E-88FC-C9D7BBB1047E}"/>
   </cellStyles>
-  <dxfs count="90">
+  <dxfs count="93">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1131,73 +1149,73 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89EE1AE9-7312-714F-B9A7-0DDE94FB0AF2}" name="segundo_neto" displayName="segundo_neto" ref="A1:S2" insertRow="1" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{89EE1AE9-7312-714F-B9A7-0DDE94FB0AF2}" name="segundo_neto" displayName="segundo_neto" ref="A1:S2" insertRow="1" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
   <autoFilter ref="A1:S2" xr:uid="{6B04083D-D905-7C42-A4F1-F7AB6E971E21}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{8105DF0A-3AF1-B245-8DE2-697A88EB4A4E}" name="id_global" dataDxfId="87"/>
-    <tableColumn id="269" xr3:uid="{B1B45D45-6AC5-4974-B8E7-2499F7127A44}" name="focalizado" dataDxfId="86"/>
-    <tableColumn id="265" xr3:uid="{E74740D2-919F-4B5D-8711-E5619A9A116E}" name="programa" dataDxfId="85"/>
-    <tableColumn id="266" xr3:uid="{E45660F1-7AD2-41E3-9F3D-51B8FC6838F2}" name="año" dataDxfId="84"/>
-    <tableColumn id="11" xr3:uid="{08A5DD2B-1EB3-E141-A58A-D2C8F7DB1899}" name="Departamento" dataDxfId="83"/>
-    <tableColumn id="12" xr3:uid="{009C0586-BAB3-B948-801C-33DC603A0A05}" name="Municipio" dataDxfId="82"/>
-    <tableColumn id="13" xr3:uid="{041FA3EE-EF40-3A42-A3BB-B393AE9404F4}" name="Colegio" dataDxfId="81"/>
-    <tableColumn id="14" xr3:uid="{819A2E74-20F8-0349-B03E-B1E83EEB7C84}" name="Sede" dataDxfId="80"/>
-    <tableColumn id="18" xr3:uid="{C9ADB558-86AF-CA40-9E31-A1A33C6DF213}" name="Género" dataDxfId="79"/>
-    <tableColumn id="22" xr3:uid="{41066F22-CAF1-0F4B-BCBB-5A53EFEC2AEA}" name="Grado" dataDxfId="78"/>
-    <tableColumn id="23" xr3:uid="{2EFCE3D4-61DE-464B-88CC-5B159EA6F48B}" name="Grupo" dataDxfId="77"/>
-    <tableColumn id="24" xr3:uid="{A75629DF-0921-5F46-959E-0D79F2C82FB1}" name="Jornada" dataDxfId="76"/>
-    <tableColumn id="164" xr3:uid="{EB9F49A4-C758-264B-93DA-FDACC7D5E677}" name="lectura_correctas" dataDxfId="75"/>
-    <tableColumn id="258" xr3:uid="{A97F3BA0-2F0C-284E-A207-A043A3B193C7}" name="comprensio_correctas" dataDxfId="74">
+    <tableColumn id="1" xr3:uid="{8105DF0A-3AF1-B245-8DE2-697A88EB4A4E}" name="id_global" dataDxfId="90"/>
+    <tableColumn id="269" xr3:uid="{B1B45D45-6AC5-4974-B8E7-2499F7127A44}" name="focalizado" dataDxfId="89"/>
+    <tableColumn id="265" xr3:uid="{E74740D2-919F-4B5D-8711-E5619A9A116E}" name="programa" dataDxfId="88"/>
+    <tableColumn id="266" xr3:uid="{E45660F1-7AD2-41E3-9F3D-51B8FC6838F2}" name="año" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{08A5DD2B-1EB3-E141-A58A-D2C8F7DB1899}" name="departamento" dataDxfId="86"/>
+    <tableColumn id="12" xr3:uid="{009C0586-BAB3-B948-801C-33DC603A0A05}" name="municipio" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{041FA3EE-EF40-3A42-A3BB-B393AE9404F4}" name="colegio" dataDxfId="84"/>
+    <tableColumn id="14" xr3:uid="{819A2E74-20F8-0349-B03E-B1E83EEB7C84}" name="sede" dataDxfId="83"/>
+    <tableColumn id="18" xr3:uid="{C9ADB558-86AF-CA40-9E31-A1A33C6DF213}" name="genero" dataDxfId="82"/>
+    <tableColumn id="22" xr3:uid="{41066F22-CAF1-0F4B-BCBB-5A53EFEC2AEA}" name="grado" dataDxfId="81"/>
+    <tableColumn id="23" xr3:uid="{2EFCE3D4-61DE-464B-88CC-5B159EA6F48B}" name="grupo" dataDxfId="80"/>
+    <tableColumn id="24" xr3:uid="{A75629DF-0921-5F46-959E-0D79F2C82FB1}" name="jornada" dataDxfId="79"/>
+    <tableColumn id="164" xr3:uid="{EB9F49A4-C758-264B-93DA-FDACC7D5E677}" name="lectura_correctas" dataDxfId="78"/>
+    <tableColumn id="258" xr3:uid="{A97F3BA0-2F0C-284E-A207-A043A3B193C7}" name="comprensio_correctas" dataDxfId="77">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="260" xr3:uid="{2B9E597F-3D00-1C4B-ABDF-C7D5C2D1F037}" name="oral_correctas" dataDxfId="73">
+    <tableColumn id="260" xr3:uid="{2B9E597F-3D00-1C4B-ABDF-C7D5C2D1F037}" name="oral_correctas" dataDxfId="76">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="268" xr3:uid="{62293502-02FF-284E-BBA6-7D06DE3E690D}" name="comparacion_correctas" dataDxfId="72">
+    <tableColumn id="268" xr3:uid="{62293502-02FF-284E-BBA6-7D06DE3E690D}" name="comparacion_correctas" dataDxfId="75">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="275" xr3:uid="{79F56C77-C863-C845-8614-6B331676483B}" name="numero_faltante_correctas" dataDxfId="71">
+    <tableColumn id="275" xr3:uid="{79F56C77-C863-C845-8614-6B331676483B}" name="numero_faltante_correctas" dataDxfId="74">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="220" xr3:uid="{DD3FACE9-0EAE-0C4A-AC5A-8BD478D00E28}" name="sumas_correctas" dataDxfId="70"/>
-    <tableColumn id="255" xr3:uid="{0D4305BF-9C5E-1D4C-9F35-D8AE7397B6BD}" name="restas_correctas" dataDxfId="69"/>
+    <tableColumn id="220" xr3:uid="{DD3FACE9-0EAE-0C4A-AC5A-8BD478D00E28}" name="sumas_correctas" dataDxfId="73"/>
+    <tableColumn id="255" xr3:uid="{0D4305BF-9C5E-1D4C-9F35-D8AE7397B6BD}" name="restas_correctas" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D11B39F-871B-034E-AD9F-95736B28F5A5}" name="tercero_neto" displayName="tercero_neto" ref="A1:T2" insertRow="1" totalsRowShown="0" headerRowDxfId="68" dataDxfId="67" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6D11B39F-871B-034E-AD9F-95736B28F5A5}" name="tercero_neto" displayName="tercero_neto" ref="A1:T2" insertRow="1" totalsRowShown="0" headerRowDxfId="71" dataDxfId="70" headerRowCellStyle="Normal 2">
   <autoFilter ref="A1:T2" xr:uid="{EFCD703A-12A7-0B4D-A78E-A09C7D84C936}"/>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{8F71DD92-7D8C-A449-96CF-CAD3E7A0026C}" name="ID" dataDxfId="66"/>
-    <tableColumn id="278" xr3:uid="{B6D9C027-30D2-40F0-BDFF-706886E5576E}" name="focalizado" dataDxfId="65"/>
-    <tableColumn id="276" xr3:uid="{AF0BAA47-15D1-4935-A11A-1ABC9232DF91}" name="programa" dataDxfId="64" dataCellStyle="Normal 2"/>
-    <tableColumn id="277" xr3:uid="{E0A93F59-843C-427E-AD3B-F41D5ADBFA15}" name="año" dataDxfId="63" dataCellStyle="Normal 2"/>
-    <tableColumn id="11" xr3:uid="{6D86FE38-DDAA-6843-AD44-8E8FF37E40DD}" name="Departamento" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{E8B8E27A-E555-4844-9788-B8A429FC487A}" name="Municipio" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{1E2D3349-A2DD-2F4B-8218-A5A75340891C}" name="Colegio" dataDxfId="60"/>
-    <tableColumn id="14" xr3:uid="{88FC1140-4C0D-AF42-8504-FC19B693BE61}" name="Sede" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{BD25A6CC-DCA2-7F4B-8012-3C5ECD0456D3}" name="Género" dataDxfId="58"/>
-    <tableColumn id="22" xr3:uid="{1CCD0497-AF52-B048-8196-39F7CA31316C}" name="Grado" dataDxfId="57"/>
-    <tableColumn id="23" xr3:uid="{74BBD92A-97B4-D749-91CA-3748DB574A5C}" name="Grupo" dataDxfId="56"/>
-    <tableColumn id="24" xr3:uid="{929A6020-E2CA-3A4F-99C5-D2449179ED22}" name="Jornada" dataDxfId="55"/>
-    <tableColumn id="164" xr3:uid="{3C02650A-8576-E240-A784-840A9C6D0C1E}" name="lectura_correctas" dataDxfId="54"/>
-    <tableColumn id="264" xr3:uid="{0C1230B1-D4C7-CD42-8DEA-044F9D2136E5}" name="comprension_correctas" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{8F71DD92-7D8C-A449-96CF-CAD3E7A0026C}" name="id_global" dataDxfId="69"/>
+    <tableColumn id="278" xr3:uid="{B6D9C027-30D2-40F0-BDFF-706886E5576E}" name="focalizado" dataDxfId="68"/>
+    <tableColumn id="276" xr3:uid="{AF0BAA47-15D1-4935-A11A-1ABC9232DF91}" name="programa" dataDxfId="67" dataCellStyle="Normal 2"/>
+    <tableColumn id="277" xr3:uid="{E0A93F59-843C-427E-AD3B-F41D5ADBFA15}" name="año" dataDxfId="66" dataCellStyle="Normal 2"/>
+    <tableColumn id="11" xr3:uid="{6D86FE38-DDAA-6843-AD44-8E8FF37E40DD}" name="departamento" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{E8B8E27A-E555-4844-9788-B8A429FC487A}" name="municipio" dataDxfId="64"/>
+    <tableColumn id="13" xr3:uid="{1E2D3349-A2DD-2F4B-8218-A5A75340891C}" name="colegio" dataDxfId="63"/>
+    <tableColumn id="14" xr3:uid="{88FC1140-4C0D-AF42-8504-FC19B693BE61}" name="sede" dataDxfId="62"/>
+    <tableColumn id="18" xr3:uid="{BD25A6CC-DCA2-7F4B-8012-3C5ECD0456D3}" name="genero" dataDxfId="61"/>
+    <tableColumn id="22" xr3:uid="{1CCD0497-AF52-B048-8196-39F7CA31316C}" name="grado" dataDxfId="60"/>
+    <tableColumn id="23" xr3:uid="{74BBD92A-97B4-D749-91CA-3748DB574A5C}" name="grupo" dataDxfId="59"/>
+    <tableColumn id="24" xr3:uid="{929A6020-E2CA-3A4F-99C5-D2449179ED22}" name="jornada" dataDxfId="58"/>
+    <tableColumn id="164" xr3:uid="{3C02650A-8576-E240-A784-840A9C6D0C1E}" name="lectura_correctas" dataDxfId="57"/>
+    <tableColumn id="264" xr3:uid="{0C1230B1-D4C7-CD42-8DEA-044F9D2136E5}" name="comprension_correctas" dataDxfId="56">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="266" xr3:uid="{36531EB9-8164-F346-A658-DC3BEC7F8DBA}" name="comprension_correctas2" dataDxfId="52">
+    <tableColumn id="266" xr3:uid="{36531EB9-8164-F346-A658-DC3BEC7F8DBA}" name="comprension_correctas2" dataDxfId="55">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="268" xr3:uid="{2DA3F259-34BB-CE43-B6CD-317DE213E2C8}" name="comparacion_correctas" dataDxfId="51">
+    <tableColumn id="268" xr3:uid="{2DA3F259-34BB-CE43-B6CD-317DE213E2C8}" name="comparacion_correctas" dataDxfId="54">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="270" xr3:uid="{1971FEE3-F47E-AD44-8B5A-DCC5C5A02F8E}" name="numero_faltante_correctas" dataDxfId="50">
+    <tableColumn id="270" xr3:uid="{1971FEE3-F47E-AD44-8B5A-DCC5C5A02F8E}" name="numero_faltante_correctas" dataDxfId="53">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="220" xr3:uid="{4B905805-845A-AB49-BF0E-3248FA45F38D}" name="sumas_correctas" dataDxfId="49"/>
-    <tableColumn id="255" xr3:uid="{C9A7D827-F7BE-D547-A9AB-020D2618F7E6}" name="restas_correctas" dataDxfId="48"/>
-    <tableColumn id="271" xr3:uid="{2DF08F61-7FBE-B141-A941-2D54F7C12560}" name="problemas_correctas" dataDxfId="47">
+    <tableColumn id="220" xr3:uid="{4B905805-845A-AB49-BF0E-3248FA45F38D}" name="sumas_correctas" dataDxfId="52"/>
+    <tableColumn id="255" xr3:uid="{C9A7D827-F7BE-D547-A9AB-020D2618F7E6}" name="restas_correctas" dataDxfId="51"/>
+    <tableColumn id="271" xr3:uid="{2DF08F61-7FBE-B141-A941-2D54F7C12560}" name="problemas_correctas" dataDxfId="50">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1206,34 +1224,34 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D19F2B2F-25BD-D04C-B5D7-8F15FC5E6887}" name="cuarto_neto" displayName="cuarto_neto" ref="A1:S2" insertRow="1" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D19F2B2F-25BD-D04C-B5D7-8F15FC5E6887}" name="cuarto_neto" displayName="cuarto_neto" ref="A1:S2" insertRow="1" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:S2" xr:uid="{245AEACF-E143-0A49-957E-A8AE7F4630F8}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{320C4EF3-3662-724F-B4F9-8B4A4956C86F}" name="ID" dataDxfId="44"/>
-    <tableColumn id="301" xr3:uid="{3E4644D9-D22D-4E07-834A-99FBF8939319}" name="focalizado" dataDxfId="43"/>
-    <tableColumn id="288" xr3:uid="{9494E8FD-8E38-4397-9EF4-4350425CD06B}" name="programa" dataDxfId="42"/>
-    <tableColumn id="300" xr3:uid="{E8230C10-BBCA-4698-91A2-5782F9E5E717}" name="año" dataDxfId="41"/>
-    <tableColumn id="11" xr3:uid="{6DF1BFCF-6C30-B044-AD39-016A6E244E28}" name="Departamento" dataDxfId="40"/>
-    <tableColumn id="12" xr3:uid="{4F54D3ED-A7E3-7745-9FDC-DBB8A62D9871}" name="Municipio" dataDxfId="39"/>
-    <tableColumn id="13" xr3:uid="{0E3E2BEC-C12C-4541-9587-18E57A1A5024}" name="Colegio" dataDxfId="38"/>
-    <tableColumn id="14" xr3:uid="{B1D6B5BF-F00D-C043-9B33-F919E65C1F94}" name="Sede" dataDxfId="37"/>
-    <tableColumn id="18" xr3:uid="{11FF5D41-B9B6-C64B-A296-422FEB690B82}" name="Género" dataDxfId="36"/>
-    <tableColumn id="22" xr3:uid="{3BBA0588-CBAA-0940-A6D5-5452F40176E0}" name="Grado" dataDxfId="35"/>
-    <tableColumn id="23" xr3:uid="{0F8DE7E1-8BB7-3A42-8677-48CB11A6FCD1}" name="Grupo" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{DCBE373C-CBC6-8941-A0A3-4CBFB01D1A01}" name="Jornada" dataDxfId="33"/>
-    <tableColumn id="196" xr3:uid="{7BB0875A-FE98-7049-9756-87750E0FD719}" name="lectura_correctas" dataDxfId="32"/>
-    <tableColumn id="290" xr3:uid="{EFA46A60-35D6-1149-A8E4-1E905B04A3D4}" name="comprension_correctas" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{320C4EF3-3662-724F-B4F9-8B4A4956C86F}" name="id_global" dataDxfId="47"/>
+    <tableColumn id="301" xr3:uid="{3E4644D9-D22D-4E07-834A-99FBF8939319}" name="focalizado" dataDxfId="46"/>
+    <tableColumn id="288" xr3:uid="{9494E8FD-8E38-4397-9EF4-4350425CD06B}" name="programa" dataDxfId="45"/>
+    <tableColumn id="300" xr3:uid="{E8230C10-BBCA-4698-91A2-5782F9E5E717}" name="año" dataDxfId="44"/>
+    <tableColumn id="11" xr3:uid="{6DF1BFCF-6C30-B044-AD39-016A6E244E28}" name="departamento" dataDxfId="43"/>
+    <tableColumn id="12" xr3:uid="{4F54D3ED-A7E3-7745-9FDC-DBB8A62D9871}" name="municipio" dataDxfId="42"/>
+    <tableColumn id="13" xr3:uid="{0E3E2BEC-C12C-4541-9587-18E57A1A5024}" name="colegio" dataDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{B1D6B5BF-F00D-C043-9B33-F919E65C1F94}" name="sede" dataDxfId="40"/>
+    <tableColumn id="18" xr3:uid="{11FF5D41-B9B6-C64B-A296-422FEB690B82}" name="genero" dataDxfId="39"/>
+    <tableColumn id="22" xr3:uid="{3BBA0588-CBAA-0940-A6D5-5452F40176E0}" name="grado" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{0F8DE7E1-8BB7-3A42-8677-48CB11A6FCD1}" name="grupo" dataDxfId="37"/>
+    <tableColumn id="24" xr3:uid="{DCBE373C-CBC6-8941-A0A3-4CBFB01D1A01}" name="jornada" dataDxfId="36"/>
+    <tableColumn id="196" xr3:uid="{7BB0875A-FE98-7049-9756-87750E0FD719}" name="lectura_correctas" dataDxfId="35"/>
+    <tableColumn id="290" xr3:uid="{EFA46A60-35D6-1149-A8E4-1E905B04A3D4}" name="comprension_correctas" dataDxfId="34">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="292" xr3:uid="{E1751D1C-F236-7949-B963-D3DBF077839B}" name="oral_correctas" dataDxfId="30">
+    <tableColumn id="292" xr3:uid="{E1751D1C-F236-7949-B963-D3DBF077839B}" name="oral_correctas" dataDxfId="33">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="294" xr3:uid="{A17D9F8A-FD82-7D49-9349-7A39F24F7C8E}" name="numero_faltante_correctas" dataDxfId="29">
+    <tableColumn id="294" xr3:uid="{A17D9F8A-FD82-7D49-9349-7A39F24F7C8E}" name="numero_faltante_correctas" dataDxfId="32">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="245" xr3:uid="{3069CBA8-A7C1-0442-B672-8B1AD69652B2}" name="sumas_correctas" dataDxfId="28"/>
-    <tableColumn id="280" xr3:uid="{2B57F784-3EBE-B645-B78A-CD39E8A81B0D}" name="restas_correctas" dataDxfId="27"/>
-    <tableColumn id="296" xr3:uid="{CB3996E5-0FE2-6242-BEC5-3F37EEBA3B5F}" name="problemas_correctas" dataDxfId="26">
+    <tableColumn id="245" xr3:uid="{3069CBA8-A7C1-0442-B672-8B1AD69652B2}" name="sumas_correctas" dataDxfId="31"/>
+    <tableColumn id="280" xr3:uid="{2B57F784-3EBE-B645-B78A-CD39E8A81B0D}" name="restas_correctas" dataDxfId="30"/>
+    <tableColumn id="296" xr3:uid="{CB3996E5-0FE2-6242-BEC5-3F37EEBA3B5F}" name="problemas_correctas" dataDxfId="29">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1242,34 +1260,34 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AC537723-3065-BB40-9020-02F6FA976B1C}" name="quinto_neto" displayName="quinto_neto" ref="A1:S2" insertRow="1" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AC537723-3065-BB40-9020-02F6FA976B1C}" name="quinto_neto" displayName="quinto_neto" ref="A1:S2" insertRow="1" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A1:S2" xr:uid="{C23A8EC1-4031-DB4F-8B54-854358EC54F8}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{287571CB-3C33-CB42-A873-842F0585EFDE}" name="ID" dataDxfId="23"/>
-    <tableColumn id="302" xr3:uid="{A82A02F1-2F33-42F7-ADD5-D88E9431C511}" name="focalizado" dataDxfId="22"/>
-    <tableColumn id="288" xr3:uid="{049971D0-363F-4735-AD80-D3031C767B3F}" name="programa" dataDxfId="21"/>
-    <tableColumn id="289" xr3:uid="{C6145414-AE26-490F-B7D7-AA2DC5DC2FA9}" name="año" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{AEA6833B-1D8B-BA42-AD3D-AFD420CD8E8A}" name="Departamento" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{4389A849-044D-EC45-A28B-E467BC1E56E1}" name="Municipio" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{F1311113-7603-C84D-9C43-25D8FFA7F55A}" name="Colegio" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{632CB065-794B-4446-8CDE-A481DC2B302A}" name="Sede" dataDxfId="16"/>
-    <tableColumn id="18" xr3:uid="{CEEC71BA-0079-1548-9201-0F59651C5880}" name="Género" dataDxfId="15"/>
-    <tableColumn id="22" xr3:uid="{189F9B64-56D9-5846-A2D2-5169D7BB903B}" name="Grado" dataDxfId="14"/>
-    <tableColumn id="23" xr3:uid="{E2B1AD46-18A5-8048-8CBE-D6E3DF61EC41}" name="Grupo" dataDxfId="13"/>
-    <tableColumn id="24" xr3:uid="{B94DDE2B-2764-3644-A873-850AF1640101}" name="Jornada" dataDxfId="12"/>
-    <tableColumn id="196" xr3:uid="{9A74BEC9-35A1-0042-854F-A59E18E3B118}" name="lectura_correctas" dataDxfId="11"/>
-    <tableColumn id="291" xr3:uid="{28EB458A-E4C2-EA4F-8EC3-D9C038804845}" name="comprension_correctas" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{287571CB-3C33-CB42-A873-842F0585EFDE}" name="id_global" dataDxfId="26"/>
+    <tableColumn id="302" xr3:uid="{A82A02F1-2F33-42F7-ADD5-D88E9431C511}" name="focalizado" dataDxfId="25"/>
+    <tableColumn id="288" xr3:uid="{049971D0-363F-4735-AD80-D3031C767B3F}" name="programa" dataDxfId="24"/>
+    <tableColumn id="289" xr3:uid="{C6145414-AE26-490F-B7D7-AA2DC5DC2FA9}" name="año" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{AEA6833B-1D8B-BA42-AD3D-AFD420CD8E8A}" name="departamento" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{4389A849-044D-EC45-A28B-E467BC1E56E1}" name="municipio" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{F1311113-7603-C84D-9C43-25D8FFA7F55A}" name="colegio" dataDxfId="20"/>
+    <tableColumn id="14" xr3:uid="{632CB065-794B-4446-8CDE-A481DC2B302A}" name="sede" dataDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{CEEC71BA-0079-1548-9201-0F59651C5880}" name="genero" dataDxfId="18"/>
+    <tableColumn id="22" xr3:uid="{189F9B64-56D9-5846-A2D2-5169D7BB903B}" name="grado" dataDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{E2B1AD46-18A5-8048-8CBE-D6E3DF61EC41}" name="grupo" dataDxfId="16"/>
+    <tableColumn id="24" xr3:uid="{B94DDE2B-2764-3644-A873-850AF1640101}" name="jornada" dataDxfId="15"/>
+    <tableColumn id="196" xr3:uid="{9A74BEC9-35A1-0042-854F-A59E18E3B118}" name="lectura_correctas" dataDxfId="14"/>
+    <tableColumn id="291" xr3:uid="{28EB458A-E4C2-EA4F-8EC3-D9C038804845}" name="comprension_correctas" dataDxfId="13">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="293" xr3:uid="{3AEDE4F0-E44F-D340-A23B-CC4F650A4144}" name="oral_correctas" dataDxfId="9">
+    <tableColumn id="293" xr3:uid="{3AEDE4F0-E44F-D340-A23B-CC4F650A4144}" name="oral_correctas" dataDxfId="12">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="295" xr3:uid="{DA0AB79B-0E6A-EE45-B565-69EAC73E2A29}" name="numero_faltante_correctas" dataDxfId="8">
+    <tableColumn id="295" xr3:uid="{DA0AB79B-0E6A-EE45-B565-69EAC73E2A29}" name="numero_faltante_correctas" dataDxfId="11">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="245" xr3:uid="{6AED42A6-1AC5-9746-A729-F3B88F4C7F97}" name="sumas_correctas" dataDxfId="7"/>
-    <tableColumn id="280" xr3:uid="{E18A5E24-3CCD-D244-8DE5-5A5054255CC5}" name="restas_correctas" dataDxfId="6"/>
-    <tableColumn id="297" xr3:uid="{DB60C108-AFF9-094E-AC02-C3CBB819B0E5}" name="problemas_correctas" dataDxfId="5">
+    <tableColumn id="245" xr3:uid="{6AED42A6-1AC5-9746-A729-F3B88F4C7F97}" name="sumas_correctas" dataDxfId="10"/>
+    <tableColumn id="280" xr3:uid="{E18A5E24-3CCD-D244-8DE5-5A5054255CC5}" name="restas_correctas" dataDxfId="9"/>
+    <tableColumn id="297" xr3:uid="{DB60C108-AFF9-094E-AC02-C3CBB819B0E5}" name="problemas_correctas" dataDxfId="8">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1278,7 +1296,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1577,74 +1595,74 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="19" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="M1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1668,7 +1686,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1682,78 +1700,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06A21148-D8A3-AF44-8FA6-AD85FFABD99F}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="20" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1777,11 +1795,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1794,75 +1815,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA110447-401E-8641-938E-3BE4826DC78E}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="19" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1886,7 +1907,10 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="1" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1899,75 +1923,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11BA45A-054A-3140-A432-C963C17C6940}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AE23" sqref="AE23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="19" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="N1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1990,7 +2014,10 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A1048576">
+  <conditionalFormatting sqref="A2:A1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2002,21 +2029,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007E6519502A214D43B3DDFCF5E94F901E" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="90f6c4560d8bc755c62d8c2203e7a644">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3eff0a0a-75ec-4759-8be4-4c323b0f0df5" xmlns:ns3="cd170719-9bd0-436b-b4b8-eee07325531c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64ddfcc38bb4a68bf603592444bf132" ns2:_="" ns3:_="">
     <xsd:import namespace="3eff0a0a-75ec-4759-8be4-4c323b0f0df5"/>
@@ -2193,24 +2205,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0697C22B-38B3-4C01-B030-F68A931777D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BF7888F-4A06-4CF8-AEBC-6002EE25BDDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E6C8263-4744-4D7D-860B-25A0C5A87C16}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2227,4 +2237,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BF7888F-4A06-4CF8-AEBC-6002EE25BDDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0697C22B-38B3-4C01-B030-F68A931777D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ultimos ajustes 20 de junio
</commit_message>
<xml_diff>
--- a/Base_organizada/BBDD_Ortial/Estructura.xlsx
+++ b/Base_organizada/BBDD_Ortial/Estructura.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danyk\OneDrive\Documents\AulaGlobalRepo\Proyecto_AulaGlobal\Base_organizada\BBDD_Ortial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bambooanalytics-my.sharepoint.com/personal/francisco_echeverri_wadua_com_co/Documents/Documentos/Prueba_GIT_AG/Proyecto_AulaGlobal/Base_organizada/BBDD_Ortial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6FE25E-F02D-442B-9D8C-54FCF53CD718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FF6FE25E-F02D-442B-9D8C-54FCF53CD718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{275FE91E-2135-4AF3-AC0F-946829A87368}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-870" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{01EC7A51-1FAE-4D41-B894-C0ABBF3FD8AA}"/>
+    <workbookView xWindow="-19320" yWindow="-2085" windowWidth="19440" windowHeight="15000" xr2:uid="{01EC7A51-1FAE-4D41-B894-C0ABBF3FD8AA}"/>
   </bookViews>
   <sheets>
     <sheet name="2º" sheetId="5" r:id="rId1"/>
@@ -39,12 +39,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="21">
   <si>
     <t>lectura_correctas</t>
-  </si>
-  <si>
-    <t>comprensio_correctas</t>
   </si>
   <si>
     <t>oral_correctas</t>
@@ -1165,7 +1162,7 @@
     <tableColumn id="23" xr3:uid="{2EFCE3D4-61DE-464B-88CC-5B159EA6F48B}" name="grupo" dataDxfId="80"/>
     <tableColumn id="24" xr3:uid="{A75629DF-0921-5F46-959E-0D79F2C82FB1}" name="jornada" dataDxfId="79"/>
     <tableColumn id="164" xr3:uid="{EB9F49A4-C758-264B-93DA-FDACC7D5E677}" name="lectura_correctas" dataDxfId="78"/>
-    <tableColumn id="258" xr3:uid="{A97F3BA0-2F0C-284E-A207-A043A3B193C7}" name="comprensio_correctas" dataDxfId="77">
+    <tableColumn id="258" xr3:uid="{A97F3BA0-2F0C-284E-A207-A043A3B193C7}" name="comprension_correctas" dataDxfId="77">
       <calculatedColumnFormula>COUNTIF(#REF!,"Correcto")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="260" xr3:uid="{2B9E597F-3D00-1C4B-ABDF-C7D5C2D1F037}" name="oral_correctas" dataDxfId="76">
@@ -1296,7 +1293,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1594,75 +1591,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CDDCABE-9E5A-2B48-B8A3-AA3AF7C72DD3}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="19" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1701,77 +1698,77 @@
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="20" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1795,14 +1792,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3:B1048576">
-    <cfRule type="duplicateValues" dxfId="5" priority="16"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="16"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1815,75 +1812,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA110447-401E-8641-938E-3BE4826DC78E}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="19" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1906,11 +1903,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="4" priority="17"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="17"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1923,75 +1920,75 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D11BA45A-054A-3140-A432-C963C17C6940}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="19" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="S1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2014,11 +2011,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2:A1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2029,6 +2026,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101007E6519502A214D43B3DDFCF5E94F901E" ma:contentTypeVersion="6" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="90f6c4560d8bc755c62d8c2203e7a644">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3eff0a0a-75ec-4759-8be4-4c323b0f0df5" xmlns:ns3="cd170719-9bd0-436b-b4b8-eee07325531c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64ddfcc38bb4a68bf603592444bf132" ns2:_="" ns3:_="">
     <xsd:import namespace="3eff0a0a-75ec-4759-8be4-4c323b0f0df5"/>
@@ -2205,22 +2217,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0697C22B-38B3-4C01-B030-F68A931777D9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BF7888F-4A06-4CF8-AEBC-6002EE25BDDD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5E6C8263-4744-4D7D-860B-25A0C5A87C16}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2237,21 +2251,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6BF7888F-4A06-4CF8-AEBC-6002EE25BDDD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0697C22B-38B3-4C01-B030-F68A931777D9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>